<commit_message>
Creacion de CSV salary
Se uso libreria en pandas para hacer el csv de salary
</commit_message>
<xml_diff>
--- a/Others/DictionaryProyect01.xlsx
+++ b/Others/DictionaryProyect01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\UVG\CODING\Semestre 4\DB1\Proyectos\Proyecto1\Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raule\Documents\GitHub\BasedeDatosProyecto1\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84401D25-7DE5-457D-AC3A-C0DCACA1930E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="2304" yWindow="1380" windowWidth="18156" windowHeight="11580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="102">
   <si>
     <t>Field</t>
   </si>
@@ -169,12 +170,6 @@
   </si>
   <si>
     <t>Player_Salary.csv</t>
-  </si>
-  <si>
-    <t>Player's type of status, if is waived, on roaster, team option, player option, non guarateed, etc. (Represented by a binary of 6 digits)</t>
-  </si>
-  <si>
-    <t>Contract_Status</t>
   </si>
   <si>
     <t>Abberviation</t>
@@ -345,7 +340,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -669,24 +664,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -726,7 +721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -746,7 +741,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -766,7 +761,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -786,7 +781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -806,7 +801,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -826,7 +821,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -846,7 +841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -866,7 +861,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -886,7 +881,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -906,7 +901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -926,7 +921,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -946,7 +941,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -972,24 +967,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1004,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1029,7 +1024,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1049,7 +1044,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1069,7 +1064,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1089,27 +1084,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6" s="3"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F7" s="1"/>
     </row>
   </sheetData>
@@ -1118,19 +1097,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1150,44 +1129,44 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1196,16 +1175,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1225,15 +1204,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1241,380 +1220,380 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="E41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>92</v>
-      </c>
-      <c r="E42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>95</v>
-      </c>
-      <c r="E45" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="E49" t="s">
         <v>96</v>
       </c>
-      <c r="E46" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>97</v>
-      </c>
-      <c r="E47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>99</v>
       </c>
-      <c r="E48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>100</v>
-      </c>
-      <c r="E49" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>101</v>
-      </c>
       <c r="E50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1623,16 +1602,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1652,14 +1631,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Creacion de tablas Teams
Generar tabla teams
</commit_message>
<xml_diff>
--- a/Others/DictionaryProyect01.xlsx
+++ b/Others/DictionaryProyect01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raule\Documents\GitHub\BasedeDatosProyecto1\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84401D25-7DE5-457D-AC3A-C0DCACA1930E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEFC586-7780-4F74-8555-7E6B2A537070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="1380" windowWidth="18156" windowHeight="11580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="780" windowWidth="18156" windowHeight="11580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="101">
   <si>
     <t>Field</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>State</t>
-  </si>
-  <si>
-    <t>Coach_Was_Player</t>
   </si>
   <si>
     <t>Arena</t>
@@ -1098,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1162,11 +1159,6 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1198,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>41</v>
@@ -1222,7 +1214,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>42</v>
@@ -1230,23 +1222,23 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
@@ -1254,7 +1246,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
         <v>42</v>
@@ -1262,7 +1254,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
         <v>42</v>
@@ -1270,7 +1262,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>42</v>
@@ -1278,7 +1270,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
@@ -1286,7 +1278,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
         <v>42</v>
@@ -1294,7 +1286,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
         <v>42</v>
@@ -1302,7 +1294,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>42</v>
@@ -1310,7 +1302,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>42</v>
@@ -1318,7 +1310,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
         <v>42</v>
@@ -1326,7 +1318,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
         <v>42</v>
@@ -1334,7 +1326,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
         <v>42</v>
@@ -1342,7 +1334,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
         <v>42</v>
@@ -1350,7 +1342,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
         <v>42</v>
@@ -1358,7 +1350,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
         <v>42</v>
@@ -1366,7 +1358,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
         <v>42</v>
@@ -1374,7 +1366,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
         <v>42</v>
@@ -1382,7 +1374,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
         <v>42</v>
@@ -1390,7 +1382,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
@@ -1398,7 +1390,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
         <v>42</v>
@@ -1406,7 +1398,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s">
         <v>42</v>
@@ -1414,7 +1406,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
         <v>42</v>
@@ -1422,7 +1414,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" t="s">
         <v>42</v>
@@ -1430,7 +1422,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
         <v>42</v>
@@ -1438,7 +1430,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" t="s">
         <v>42</v>
@@ -1446,7 +1438,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" t="s">
         <v>42</v>
@@ -1454,7 +1446,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s">
         <v>42</v>
@@ -1462,7 +1454,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
         <v>42</v>
@@ -1470,7 +1462,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E35" t="s">
         <v>42</v>
@@ -1478,7 +1470,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" t="s">
         <v>42</v>
@@ -1486,7 +1478,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" t="s">
         <v>42</v>
@@ -1494,7 +1486,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E38" t="s">
         <v>42</v>
@@ -1502,7 +1494,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39" t="s">
         <v>42</v>
@@ -1510,7 +1502,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
         <v>42</v>
@@ -1518,7 +1510,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E41" t="s">
         <v>42</v>
@@ -1526,7 +1518,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
         <v>42</v>
@@ -1534,7 +1526,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
         <v>42</v>
@@ -1542,7 +1534,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E44" t="s">
         <v>42</v>
@@ -1550,7 +1542,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E45" t="s">
         <v>42</v>
@@ -1558,7 +1550,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E46" t="s">
         <v>42</v>
@@ -1566,7 +1558,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E47" t="s">
         <v>42</v>
@@ -1574,26 +1566,26 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1633,12 +1625,12 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Primer intento de insercion de datos
Primer intento de insercion
</commit_message>
<xml_diff>
--- a/Others/DictionaryProyect01.xlsx
+++ b/Others/DictionaryProyect01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raule\Documents\GitHub\BasedeDatosProyecto1\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768FCBE3-ABB4-48AC-AB51-9BFA060731B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA244707-9C28-4C79-9BCA-6C42E98896A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="780" windowWidth="18156" windowHeight="11580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="165">
   <si>
     <t>Field</t>
   </si>
@@ -172,9 +172,6 @@
     <t>Player_Salary.csv</t>
   </si>
   <si>
-    <t>Abberviation</t>
-  </si>
-  <si>
     <t>Nickname</t>
   </si>
   <si>
@@ -521,6 +518,12 @@
   </si>
   <si>
     <t>Name of game official</t>
+  </si>
+  <si>
+    <t>fk</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
   </si>
 </sst>
 </file>
@@ -854,7 +857,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,7 +1004,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
@@ -1156,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,7 +1218,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1224,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="F3" t="s">
         <v>33</v>
@@ -1287,7 +1290,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,13 +1329,13 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
         <v>103</v>
       </c>
-      <c r="E2" t="s">
-        <v>104</v>
-      </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1340,119 +1343,119 @@
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3">
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8">
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1492,7 +1495,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1501,13 +1504,13 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
         <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1521,18 +1524,18 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1541,18 +1544,18 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
         <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1561,18 +1564,18 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -1581,18 +1584,18 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -1601,18 +1604,18 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1621,18 +1624,18 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" t="s">
         <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -1641,18 +1644,18 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s">
         <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -1661,18 +1664,18 @@
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
         <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -1681,18 +1684,18 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -1701,18 +1704,18 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
         <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -1721,18 +1724,18 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E13" t="s">
         <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1741,18 +1744,18 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
         <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1761,18 +1764,18 @@
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
         <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -1781,18 +1784,18 @@
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
         <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -1801,18 +1804,18 @@
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E17" t="s">
         <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -1821,18 +1824,18 @@
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E18" t="s">
         <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -1841,18 +1844,18 @@
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
         <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -1861,18 +1864,18 @@
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E20" t="s">
         <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
@@ -1881,18 +1884,18 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E21" t="s">
         <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1901,18 +1904,18 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E22" t="s">
         <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
@@ -1921,18 +1924,18 @@
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
         <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
@@ -1941,18 +1944,18 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E24" t="s">
         <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -1961,18 +1964,18 @@
         <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -1981,18 +1984,18 @@
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E26" t="s">
         <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -2001,18 +2004,18 @@
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" t="s">
         <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -2021,18 +2024,18 @@
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E28" t="s">
         <v>42</v>
       </c>
       <c r="F28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
@@ -2041,18 +2044,18 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E29" t="s">
         <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -2061,18 +2064,18 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" t="s">
         <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
@@ -2081,18 +2084,18 @@
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E31" t="s">
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
@@ -2101,18 +2104,18 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E32" t="s">
         <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
@@ -2121,18 +2124,18 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E33" t="s">
         <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
@@ -2141,18 +2144,18 @@
         <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
@@ -2161,18 +2164,18 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E35" t="s">
         <v>42</v>
       </c>
       <c r="F35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
@@ -2181,18 +2184,18 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E36" t="s">
         <v>42</v>
       </c>
       <c r="F36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
@@ -2201,18 +2204,18 @@
         <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E37" t="s">
         <v>42</v>
       </c>
       <c r="F37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
@@ -2221,18 +2224,18 @@
         <v>20</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E38" t="s">
         <v>42</v>
       </c>
       <c r="F38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
@@ -2241,18 +2244,18 @@
         <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E39" t="s">
         <v>42</v>
       </c>
       <c r="F39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
@@ -2261,18 +2264,18 @@
         <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E40" t="s">
         <v>42</v>
       </c>
       <c r="F40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
@@ -2281,18 +2284,18 @@
         <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E41" t="s">
         <v>42</v>
       </c>
       <c r="F41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
@@ -2301,18 +2304,18 @@
         <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E42" t="s">
         <v>42</v>
       </c>
       <c r="F42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
@@ -2321,18 +2324,18 @@
         <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E43" t="s">
         <v>42</v>
       </c>
       <c r="F43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
@@ -2341,18 +2344,18 @@
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E44" t="s">
         <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
@@ -2361,18 +2364,18 @@
         <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E45" t="s">
         <v>42</v>
       </c>
       <c r="F45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
@@ -2381,18 +2384,18 @@
         <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E46" t="s">
         <v>42</v>
       </c>
       <c r="F46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
@@ -2401,18 +2404,18 @@
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E47" t="s">
         <v>42</v>
       </c>
       <c r="F47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
@@ -2421,18 +2424,18 @@
         <v>20</v>
       </c>
       <c r="D48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
@@ -2441,18 +2444,18 @@
         <v>20</v>
       </c>
       <c r="D49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
@@ -2461,13 +2464,13 @@
         <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2479,7 +2482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="F46" sqref="F46:F47"/>
     </sheetView>
   </sheetViews>
@@ -2507,12 +2510,12 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="2"/>
     </row>
@@ -2538,7 +2541,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -2547,13 +2550,13 @@
         <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2561,19 +2564,19 @@
         <v>34</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C47">
         <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E47" t="s">
         <v>42</v>
       </c>
       <c r="F47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creacion de todas las tablas excepto la juegos
Creacion desde python las tablas a utilizar
</commit_message>
<xml_diff>
--- a/Others/DictionaryProyect01.xlsx
+++ b/Others/DictionaryProyect01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raule\Documents\GitHub\BasedeDatosProyecto1\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA244707-9C28-4C79-9BCA-6C42E98896A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA535CA7-DBE0-4D8F-BC43-05A75DC31D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="780" windowWidth="18156" windowHeight="11580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="780" windowWidth="18156" windowHeight="11580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -1159,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1218,7 +1218,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1467,7 +1467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -2482,7 +2482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
       <selection activeCell="F46" sqref="F46:F47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates Diego 1 AM
</commit_message>
<xml_diff>
--- a/Others/DictionaryProyect01.xlsx
+++ b/Others/DictionaryProyect01.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raule\Documents\GitHub\BasedeDatosProyecto1\Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\UVG\CODING\Semestre 4\DB1\Proyectos\Proyecto1\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768FCBE3-ABB4-48AC-AB51-9BFA060731B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="166">
   <si>
     <t>Field</t>
   </si>
@@ -521,12 +520,18 @@
   </si>
   <si>
     <t>Name of game official</t>
+  </si>
+  <si>
+    <t>Arena_Capacity</t>
+  </si>
+  <si>
+    <t>Arena's capacity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -850,24 +855,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -887,7 +892,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -907,7 +912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -927,7 +932,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -947,7 +952,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -967,7 +972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -987,7 +992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1007,7 +1012,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1047,7 +1052,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1067,7 +1072,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1087,7 +1092,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1107,7 +1112,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1127,7 +1132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1153,24 +1158,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1210,7 +1215,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1230,7 +1235,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1250,7 +1255,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1270,11 +1275,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F7" s="1"/>
     </row>
   </sheetData>
@@ -1283,19 +1288,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1320,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1335,7 +1340,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1355,7 +1360,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1375,7 +1380,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1395,7 +1400,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1415,7 +1420,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1435,7 +1440,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1455,22 +1460,43 @@
         <v>108</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1490,7 +1516,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1510,7 +1536,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1530,7 +1556,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1550,7 +1576,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1570,7 +1596,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1590,7 +1616,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1610,7 +1636,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1630,7 +1656,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1650,7 +1676,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1670,7 +1696,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1690,7 +1716,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -1710,7 +1736,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1730,7 +1756,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1750,7 +1776,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1770,7 +1796,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1790,7 +1816,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1810,7 +1836,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1830,7 +1856,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -1850,7 +1876,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1870,7 +1896,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1890,7 +1916,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -1910,7 +1936,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -1930,7 +1956,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -1950,7 +1976,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -1970,7 +1996,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -1990,7 +2016,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -2010,7 +2036,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2030,7 +2056,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -2050,7 +2076,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -2070,7 +2096,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -2090,7 +2116,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -2110,7 +2136,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2130,7 +2156,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -2150,7 +2176,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2170,7 +2196,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2190,7 +2216,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -2210,7 +2236,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -2230,7 +2256,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -2250,7 +2276,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2270,7 +2296,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2290,7 +2316,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2310,7 +2336,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -2330,7 +2356,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2350,7 +2376,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -2370,7 +2396,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -2390,7 +2416,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -2410,7 +2436,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -2430,7 +2456,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -2450,7 +2476,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2476,16 +2502,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46:F47"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2505,18 +2531,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2536,7 +2562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -2556,7 +2582,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Made the entity relationship diagram
</commit_message>
<xml_diff>
--- a/Others/DictionaryProyect01.xlsx
+++ b/Others/DictionaryProyect01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="173">
   <si>
     <t>Field</t>
   </si>
@@ -541,6 +541,12 @@
   </si>
   <si>
     <t>Coach_was_Player</t>
+  </si>
+  <si>
+    <t>Status_Player</t>
+  </si>
+  <si>
+    <t>Player's status if it's active or inactive</t>
   </si>
 </sst>
 </file>
@@ -871,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,6 +1170,26 @@
         <v>42</v>
       </c>
       <c r="F14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1525,7 +1551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>